<commit_message>
Software Versions.xlsx incorrectly listed the python version and is now fixed.
</commit_message>
<xml_diff>
--- a/docs/Software Versions.xlsx
+++ b/docs/Software Versions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/jcslack_ad_unc_edu/Documents/Open-Source Operant Chamber Methods Paper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slack\Github\open-source-rat-behavior\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="11_F25DC773A252ABDACC1048A3D11B50905BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A14B595A-7AF4-469E-9F18-7E8F197BA809}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25130B9-9FE5-4713-8B93-749C30C48B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>Python/IDLE</t>
   </si>
   <si>
-    <t>2.8.3rc1</t>
-  </si>
-  <si>
     <t>Arduino IDE</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>&gt;=2.39.1</t>
+  </si>
+  <si>
+    <t>3.8.3rc1</t>
   </si>
 </sst>
 </file>
@@ -174,11 +174,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3B74A66D-AFFE-4487-AE98-C602CF3366DB}" name="Table1" displayName="Table1" ref="A1:B10" totalsRowShown="0" headerRowDxfId="3" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3B74A66D-AFFE-4487-AE98-C602CF3366DB}" name="Table1" displayName="Table1" ref="A1:B10" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A1:B10" xr:uid="{3B74A66D-AFFE-4487-AE98-C602CF3366DB}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F76B2AD7-CA91-4B61-A842-C4CA9851E965}" name="Software" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{34A24BA2-2351-46CC-984D-D4FB74779A8E}" name="Version" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{F76B2AD7-CA91-4B61-A842-C4CA9851E965}" name="Software" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{34A24BA2-2351-46CC-984D-D4FB74779A8E}" name="Version" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -450,7 +450,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -472,7 +472,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -488,20 +488,20 @@
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2">
         <v>1.36</v>
@@ -509,15 +509,15 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2">
         <v>1.97</v>
@@ -525,18 +525,18 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added batch files for automatically running frontend and backend. Updated README and verified a few python/package versioning requirements.
</commit_message>
<xml_diff>
--- a/docs/Software Versions.xlsx
+++ b/docs/Software Versions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slack\Github\open-source-rat-behavior\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25130B9-9FE5-4713-8B93-749C30C48B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A78A0B-4F33-4662-B86A-67D6D376358D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
     <t>&gt;=2.39.1</t>
   </si>
   <si>
-    <t>3.8.3rc1</t>
+    <t>3.8.10 (Initial development on 3.8.3rc1)</t>
   </si>
 </sst>
 </file>
@@ -450,13 +450,13 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.5546875" customWidth="1"/>
-    <col min="2" max="2" width="30.5546875" customWidth="1"/>
+    <col min="2" max="2" width="34.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>